<commit_message>
skull stripping and evaluation snippits
</commit_message>
<xml_diff>
--- a/Lab 1/dice results.xlsx
+++ b/Lab 1/dice results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdal\Documents\Master\EMJMD MAIA\SEMESTER 3 - UdG\MISA\Labs\Lab 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FC4D37-15CF-4803-9A2E-F3099839BB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A21C88E-65D8-442E-A809-D8AE78B14D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,7 +461,7 @@
   <dimension ref="B9:AK29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF27" sqref="AF27"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>